<commit_message>
Update MS account mappings in Mappings.xlsx.
</commit_message>
<xml_diff>
--- a/aurum_backend/data/excel/input_files/Mappings.xlsx
+++ b/aurum_backend/data/excel/input_files/Mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaskemeny/AurumFinanceAI/aurum_backend/data/excel/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD468CD8-5C88-B842-9E7D-352FB0DD94C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2679827-08AF-2342-84AF-39DA83E921C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="1140" windowWidth="23060" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="1140" windowWidth="23060" windowHeight="14200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JPM" sheetId="1" r:id="rId1"/>
@@ -691,52 +691,52 @@
     <t>Velero</t>
   </si>
   <si>
-    <t>Cardor Alef SpA - 4597</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime - 4231</t>
-  </si>
-  <si>
-    <t>NNW Capital SpA - 4757</t>
-  </si>
-  <si>
-    <t>NNW II Capital SpA - 4751</t>
-  </si>
-  <si>
-    <t>FNW Capital SpA - 4756</t>
-  </si>
-  <si>
-    <t>Alanseb LP - 4582</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Felipe - 4228</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Irene - 4441</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime y Felipe - 4191</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime y Natalia - 4192</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime y Nicolas - 4190</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Natalia - 4229</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Nicolas - 4230</t>
-  </si>
-  <si>
-    <t>NNW Ventures LLC - 4357</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jacques - 4442</t>
-  </si>
-  <si>
     <t xml:space="preserve">JOHANN PETER UNGAR UNGAR </t>
+  </si>
+  <si>
+    <t>Cardor Alef SpA - 4165</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime - 4120</t>
+  </si>
+  <si>
+    <t>NNW Capital SpA - 4105</t>
+  </si>
+  <si>
+    <t>NNW II Capital SpA - 4103</t>
+  </si>
+  <si>
+    <t>FNW Capital SpA - 4157</t>
+  </si>
+  <si>
+    <t>Alanseb LP - 4156</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Felipe - 4122</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Irene - 4162</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime y Felipe - 4114</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime y Natalia - 4118</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime y Nicolas - 4121</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Natalia - 4108</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Nicolas - 4110</t>
+  </si>
+  <si>
+    <t>NNW Ventures LLC - 4107</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jacques - 4155</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -1506,7 +1506,7 @@
         <v>96</v>
       </c>
       <c r="D32" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E32" s="1"/>
     </row>
@@ -1888,8 +1888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B10" t="s">
         <v>172</v>
@@ -2015,7 +2015,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -2048,7 +2048,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
@@ -2059,7 +2059,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
@@ -2081,7 +2081,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
mappings file old for 31_07_2025.
</commit_message>
<xml_diff>
--- a/aurum_backend/data/excel/input_files/Mappings.xlsx
+++ b/aurum_backend/data/excel/input_files/Mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaskemeny/AurumFinanceAI/aurum_backend/data/excel/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2679827-08AF-2342-84AF-39DA83E921C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E92458-0F66-9544-9CD2-72802D2694EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="1140" windowWidth="23060" windowHeight="14200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,49 +694,49 @@
     <t xml:space="preserve">JOHANN PETER UNGAR UNGAR </t>
   </si>
   <si>
-    <t>Cardor Alef SpA - 4165</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime - 4120</t>
-  </si>
-  <si>
-    <t>NNW Capital SpA - 4105</t>
-  </si>
-  <si>
-    <t>NNW II Capital SpA - 4103</t>
-  </si>
-  <si>
-    <t>FNW Capital SpA - 4157</t>
-  </si>
-  <si>
-    <t>Alanseb LP - 4156</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Felipe - 4122</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Irene - 4162</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime y Felipe - 4114</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime y Natalia - 4118</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime y Nicolas - 4121</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Natalia - 4108</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Nicolas - 4110</t>
-  </si>
-  <si>
-    <t>NNW Ventures LLC - 4107</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jacques - 4155</t>
+    <t>Cardor Alef SpA - 4597</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime - 4231</t>
+  </si>
+  <si>
+    <t>NNW Capital SpA - 4757</t>
+  </si>
+  <si>
+    <t>NNW II Capital SpA - 4751</t>
+  </si>
+  <si>
+    <t>FNW Capital SpA - 4756</t>
+  </si>
+  <si>
+    <t>Alanseb LP - 4582</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Felipe - 4228</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Irene - 4441</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime y Felipe - 4191</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime y Natalia - 4192</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime y Nicolas - 4190</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Natalia - 4229</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Nicolas - 4230</t>
+  </si>
+  <si>
+    <t>NNW Ventures LLC - 4357</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jacques - 4442</t>
   </si>
 </sst>
 </file>
@@ -1889,7 +1889,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A2" sqref="A2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed mappings for 07_08_2025.
</commit_message>
<xml_diff>
--- a/aurum_backend/data/excel/input_files/Mappings.xlsx
+++ b/aurum_backend/data/excel/input_files/Mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaskemeny/AurumFinanceAI/aurum_backend/data/excel/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E92458-0F66-9544-9CD2-72802D2694EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3C8900-D7E0-6241-ACBC-AF3D10EC9237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="1140" windowWidth="23060" windowHeight="14200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,49 +694,49 @@
     <t xml:space="preserve">JOHANN PETER UNGAR UNGAR </t>
   </si>
   <si>
-    <t>Cardor Alef SpA - 4597</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime - 4231</t>
-  </si>
-  <si>
-    <t>NNW Capital SpA - 4757</t>
-  </si>
-  <si>
-    <t>NNW II Capital SpA - 4751</t>
-  </si>
-  <si>
-    <t>FNW Capital SpA - 4756</t>
-  </si>
-  <si>
-    <t>Alanseb LP - 4582</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Felipe - 4228</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Irene - 4441</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime y Felipe - 4191</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime y Natalia - 4192</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jaime y Nicolas - 4190</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Natalia - 4229</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Nicolas - 4230</t>
-  </si>
-  <si>
-    <t>NNW Ventures LLC - 4357</t>
-  </si>
-  <si>
-    <t>Cuenta Personal - Jacques - 4442</t>
+    <t>Cardor Alef SpA - 4165</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime - 4120</t>
+  </si>
+  <si>
+    <t>NNW Capital SpA - 4105</t>
+  </si>
+  <si>
+    <t>NNW II Capital SpA - 4103</t>
+  </si>
+  <si>
+    <t>FNW Capital SpA - 4157</t>
+  </si>
+  <si>
+    <t>Alanseb LP - 4156</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Felipe - 4122</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Irene - 4162</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime y Felipe - 4114</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime y Natalia - 4118</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jaime y Nicolas - 4121</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Natalia - 4108</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Nicolas - 4110</t>
+  </si>
+  <si>
+    <t>NNW Ventures LLC - 4107</t>
+  </si>
+  <si>
+    <t>Cuenta Personal - Jacques - 4155</t>
   </si>
 </sst>
 </file>
@@ -1889,7 +1889,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D21"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added Citi Bank transformer.
</commit_message>
<xml_diff>
--- a/aurum_backend/data/excel/input_files/Mappings.xlsx
+++ b/aurum_backend/data/excel/input_files/Mappings.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaskemeny/AurumFinanceAI/aurum_backend/data/excel/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101617F7-FB84-2A4E-A9D8-6FF8427162A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF570149-EDAA-F742-A347-4C0603896906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1640" windowWidth="23060" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33180" yWindow="320" windowWidth="23060" windowHeight="14200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JPM" sheetId="1" r:id="rId1"/>
-    <sheet name="MS" sheetId="2" r:id="rId2"/>
-    <sheet name="HSBC" sheetId="3" r:id="rId3"/>
-    <sheet name="LO" sheetId="4" r:id="rId4"/>
-    <sheet name="Safra" sheetId="5" r:id="rId5"/>
-    <sheet name="Banchile" sheetId="6" r:id="rId6"/>
-    <sheet name="Alternatives" sheetId="7" r:id="rId7"/>
+    <sheet name="Citi" sheetId="8" r:id="rId2"/>
+    <sheet name="MS" sheetId="2" r:id="rId3"/>
+    <sheet name="HSBC" sheetId="3" r:id="rId4"/>
+    <sheet name="LO" sheetId="4" r:id="rId5"/>
+    <sheet name="Safra" sheetId="5" r:id="rId6"/>
+    <sheet name="Banchile" sheetId="6" r:id="rId7"/>
+    <sheet name="Alternatives" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="257">
   <si>
     <t>account number</t>
   </si>
@@ -740,6 +741,63 @@
   </si>
   <si>
     <t xml:space="preserve">JOHANN P U UNGAR TOD ANDRES D U U </t>
+  </si>
+  <si>
+    <t>55EXXXX29000</t>
+  </si>
+  <si>
+    <t>55EXXXX70000</t>
+  </si>
+  <si>
+    <t>55EXXXX95000</t>
+  </si>
+  <si>
+    <t>55EXXXX99000</t>
+  </si>
+  <si>
+    <t>C75XXX131</t>
+  </si>
+  <si>
+    <t>C75XXX751</t>
+  </si>
+  <si>
+    <t>XXXX1802</t>
+  </si>
+  <si>
+    <t>XXXX1803</t>
+  </si>
+  <si>
+    <t>XXXX5752</t>
+  </si>
+  <si>
+    <t>XXXXXX9482</t>
+  </si>
+  <si>
+    <t>XXXXXX8419</t>
+  </si>
+  <si>
+    <t>KETTY</t>
+  </si>
+  <si>
+    <t>PARA</t>
+  </si>
+  <si>
+    <t>transactions_account_number</t>
+  </si>
+  <si>
+    <t>C75009131</t>
+  </si>
+  <si>
+    <t>55E307570000</t>
+  </si>
+  <si>
+    <t>55E406695000</t>
+  </si>
+  <si>
+    <t>55E397899000</t>
+  </si>
+  <si>
+    <t>C75004751</t>
   </si>
 </sst>
 </file>
@@ -775,8 +833,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1093,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1887,6 +1946,193 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FBAA79-82B9-F440-83FB-CB3F81B44D95}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>38451802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>250</v>
+      </c>
+      <c r="E10">
+        <v>10415752</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11">
+        <v>6866909482</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>9995698419</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -2141,7 +2387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2214,7 +2460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -2299,7 +2545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2350,7 +2596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -2436,7 +2682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6DDF85-D422-594C-A992-5626F2F9979A}">
   <dimension ref="A1:B38"/>
   <sheetViews>

</xml_diff>

<commit_message>
Finished implementing Bond Maturity Report, updated Mappings Citi sheet.
</commit_message>
<xml_diff>
--- a/aurum_backend/data/excel/input_files/Mappings.xlsx
+++ b/aurum_backend/data/excel/input_files/Mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaskemeny/AurumFinanceAI/aurum_backend/data/excel/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF570149-EDAA-F742-A347-4C0603896906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9E5E8C-AA35-B74B-81DA-85FFE60D0468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33180" yWindow="320" windowWidth="23060" windowHeight="14200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="247">
   <si>
     <t>account number</t>
   </si>
@@ -744,36 +744,6 @@
   </si>
   <si>
     <t>55EXXXX29000</t>
-  </si>
-  <si>
-    <t>55EXXXX70000</t>
-  </si>
-  <si>
-    <t>55EXXXX95000</t>
-  </si>
-  <si>
-    <t>55EXXXX99000</t>
-  </si>
-  <si>
-    <t>C75XXX131</t>
-  </si>
-  <si>
-    <t>C75XXX751</t>
-  </si>
-  <si>
-    <t>XXXX1802</t>
-  </si>
-  <si>
-    <t>XXXX1803</t>
-  </si>
-  <si>
-    <t>XXXX5752</t>
-  </si>
-  <si>
-    <t>XXXXXX9482</t>
-  </si>
-  <si>
-    <t>XXXXXX8419</t>
   </si>
   <si>
     <t>KETTY</t>
@@ -1950,7 +1920,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1976,7 +1946,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1991,8 +1961,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>239</v>
+      <c r="A3" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -2001,35 +1971,35 @@
         <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>240</v>
+      <c r="A4" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>241</v>
+      <c r="A5" s="1" t="s">
+        <v>245</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2043,12 +2013,12 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>243</v>
+      <c r="A7" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -2057,12 +2027,12 @@
         <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>244</v>
+      <c r="A8">
+        <v>38451802</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -2075,47 +2045,44 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>245</v>
-      </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>246</v>
+      <c r="A10">
+        <v>10415752</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="E10">
         <v>10415752</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>247</v>
+      <c r="A11">
+        <v>6866909482</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="E11">
         <v>6866909482</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>248</v>
+      <c r="A12">
+        <v>9995698419</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Update Mappings.xlsx. Have to test full EI STDSZ addition.
</commit_message>
<xml_diff>
--- a/aurum_backend/data/excel/input_files/Mappings.xlsx
+++ b/aurum_backend/data/excel/input_files/Mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaskemeny/AurumFinanceAI/aurum_backend/data/excel/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9E5E8C-AA35-B74B-81DA-85FFE60D0468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27650DED-4282-A449-8758-39E55F603AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33180" yWindow="320" windowWidth="23060" windowHeight="14200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32580" yWindow="-700" windowWidth="23060" windowHeight="14200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JPM" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="248">
   <si>
     <t>account number</t>
   </si>
@@ -743,9 +743,6 @@
     <t xml:space="preserve">JOHANN P U UNGAR TOD ANDRES D U U </t>
   </si>
   <si>
-    <t>55EXXXX29000</t>
-  </si>
-  <si>
     <t>KETTY</t>
   </si>
   <si>
@@ -768,6 +765,12 @@
   </si>
   <si>
     <t>C75004751</t>
+  </si>
+  <si>
+    <t>55E411729000</t>
+  </si>
+  <si>
+    <t>AAA - 6615</t>
   </si>
 </sst>
 </file>
@@ -803,9 +806,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1919,8 +1925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FBAA79-82B9-F440-83FB-CB3F81B44D95}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1946,12 +1952,12 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>238</v>
+      <c r="A2" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -1959,10 +1965,13 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -1971,40 +1980,40 @@
         <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -2013,12 +2022,12 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -2027,7 +2036,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2049,7 +2058,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2060,7 +2069,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E10">
         <v>10415752</v>
@@ -2074,7 +2083,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E11">
         <v>6866909482</v>
@@ -2101,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2347,6 +2356,17 @@
       </c>
       <c r="C21" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>